<commit_message>
Dropdown list for spreadsheet
and minor syntax corrections
</commit_message>
<xml_diff>
--- a/layout_tpl.xlsx
+++ b/layout_tpl.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>m</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -41,6 +41,7 @@
           <t xml:space="preserve">button
 entry
 label
+message
 scrollx
 scrolly
 list
@@ -130,7 +131,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>m</author>
   </authors>
   <commentList>
     <comment ref="A2" authorId="0">
@@ -145,6 +146,7 @@
           <t xml:space="preserve">button
 entry
 label
+message
 scrollx
 scrolly
 list
@@ -232,7 +234,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>m</author>
   </authors>
   <commentList>
     <comment ref="C2" authorId="0">
@@ -283,7 +285,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="184">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -343,6 +345,18 @@
 Attributes
 And
 Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">progress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combo</t>
   </si>
   <si>
     <t xml:space="preserve">begmenu</t>
@@ -527,10 +541,13 @@
     <t xml:space="preserve">2</t>
   </si>
   <si>
-    <t xml:space="preserve">resume parent variable name for the submenu parent _label name</t>
+    <t xml:space="preserve">parent variable name for the submenu parent _label name</t>
   </si>
   <si>
     <t xml:space="preserve">_Edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent variable name for top menu</t>
   </si>
   <si>
     <t xml:space="preserve">mn_help</t>
@@ -570,9 +587,6 @@
 Values</t>
   </si>
   <si>
-    <t xml:space="preserve">button</t>
-  </si>
-  <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
@@ -582,9 +596,6 @@
     <t xml:space="preserve">( x,x,x,… )</t>
   </si>
   <si>
-    <t xml:space="preserve">entry</t>
-  </si>
-  <si>
     <t xml:space="preserve">(x)</t>
   </si>
   <si>
@@ -630,9 +641,6 @@
     <t xml:space="preserve">x999</t>
   </si>
   <si>
-    <t xml:space="preserve">combo</t>
-  </si>
-  <si>
     <t xml:space="preserve">notebook</t>
   </si>
   <si>
@@ -657,7 +665,7 @@
     <t xml:space="preserve">999x999</t>
   </si>
   <si>
-    <t xml:space="preserve">progress</t>
+    <t xml:space="preserve">Note some of the code inserted for certain widgets is mostly “commented” out because of certain choices and modifications that will be needed.</t>
   </si>
   <si>
     <t xml:space="preserve">Widgets</t>
@@ -926,7 +934,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1024,6 +1032,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1045,6 +1068,12 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
@@ -1104,7 +1133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1127,6 +1156,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="hair"/>
@@ -1159,7 +1195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1244,7 +1280,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1280,15 +1324,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1296,31 +1340,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1332,39 +1376,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="22" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1433,7 +1481,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -1453,25 +1501,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="2" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="5.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="6.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="10.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="47.37"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="16.53"/>
   </cols>
@@ -1530,17 +1578,63 @@
       </c>
     </row>
     <row r="3" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
+      <c r="A3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:F1"/>
   </mergeCells>
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A100" type="list">
+      <formula1>"begmenu,button,check,clip,combo,endmenu,entry,filedialog,frame,geometry,label,list,message,messagebox,notebook,options,popup,progress,radio,scrollx,scrolly,spin,submenu,text"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A3" type="list">
+      <formula1>"begmenu,button,check,clip,combo,endmenu,entry,filedialog,frame,geometry,label,list,message,messagebox,notebook,options,popup,progress,radio,scrollx,scrolly,spin,submenu,text"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:H100" type="whole">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" prompt="Use N S E W&#10;in combinations.&#10;N = North&#10;S = South&#10;E = East&#10;W = West&#10;&#10;eg. NS will stretch from top to bottom of the cell&#10;eg. SW will place in the botton left corner&#10;eg. NSEW will stetch to fill all of cell&#10;" promptTitle="sticky attribute" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I3:I100" type="textLength">
+      <formula1>0</formula1>
+      <formula2>4</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1560,16 +1654,16 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="15" width="75.03"/>
   </cols>
   <sheetData>
@@ -1591,235 +1685,241 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" s="4" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="4" customFormat="true" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F2" s="16"/>
     </row>
     <row r="3" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F5" s="19"/>
     </row>
     <row r="6" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>22</v>
       </c>
       <c r="F6" s="19"/>
     </row>
     <row r="7" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F7" s="19"/>
     </row>
     <row r="8" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F8" s="19"/>
     </row>
     <row r="9" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F9" s="19"/>
     </row>
     <row r="10" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="17" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F11" s="19"/>
     </row>
     <row r="12" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>53</v>
+      <c r="B15" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F17" s="19"/>
     </row>
     <row r="18" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F18" s="19"/>
     </row>
     <row r="19" s="17" customFormat="true" ht="16.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F19" s="19"/>
     </row>
     <row r="20" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F20" s="19"/>
     </row>
@@ -1844,20 +1944,20 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="21" width="20.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="22" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="23" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="6.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="5.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="22" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="22" width="4.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="22" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="6.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="5.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="24" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="24" width="4.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="24" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.09"/>
   </cols>
   <sheetData>
@@ -1882,618 +1982,609 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="29" customFormat="true" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="23" t="s">
+    <row r="2" s="31" customFormat="true" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" s="33" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>69</v>
+      <c r="J2" s="30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" s="35" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>69</v>
+      <c r="A4" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>69</v>
+      <c r="B5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="40"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="40"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="35" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="38"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="38"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I9" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J11" s="36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="36" t="s">
-        <v>69</v>
+      <c r="E12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="38"/>
+      <c r="E13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J14" s="36" t="s">
-        <v>69</v>
+      <c r="A14" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="36" t="s">
-        <v>69</v>
+      <c r="A15" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
+      <c r="A16" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="38"/>
+      <c r="A17" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
+      <c r="A18" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="38"/>
+      <c r="A19" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="42"/>
+      <c r="A20" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="38"/>
+      <c r="A21" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="H22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="36" t="s">
-        <v>69</v>
+      <c r="A22" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="39"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="36"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="36"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="36"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+    </row>
+    <row r="24" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="38"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="36"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="36"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="36"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="36"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="36"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="36"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="36"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="36"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
-    </row>
+      <c r="A28" s="38"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
@@ -2518,216 +2609,216 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="22.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="96.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="44" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="22.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="96.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="47" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>97</v>
+      <c r="A1" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>99</v>
+      <c r="A2" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>101</v>
+      <c r="A3" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>103</v>
+      <c r="A4" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>105</v>
+      <c r="A5" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>107</v>
+      <c r="A6" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>109</v>
+      <c r="A7" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>111</v>
+      <c r="A8" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>113</v>
+      <c r="A9" s="50" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47" t="s">
-        <v>114</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>115</v>
+      <c r="A10" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="48" t="s">
+      <c r="A11" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" s="51" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="48" t="s">
-        <v>115</v>
-      </c>
-    </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>120</v>
+      <c r="A13" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>122</v>
+      <c r="A14" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>124</v>
+      <c r="A15" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>126</v>
+      <c r="A16" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>128</v>
+      <c r="A17" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="49"/>
+      <c r="A18" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="52"/>
     </row>
     <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>131</v>
+      <c r="A19" s="50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="B20" s="48" t="s">
-        <v>133</v>
+      <c r="A20" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>135</v>
+      <c r="A21" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="47" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>137</v>
+      <c r="A22" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>139</v>
+      <c r="A23" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>141</v>
+      <c r="A24" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" s="51" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="50"/>
+      <c r="A25" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" s="54" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2814,10 +2905,10 @@
     </row>
     <row r="2" s="11" customFormat="true" ht="102.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>8</v>
@@ -2831,31 +2922,31 @@
       <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="55" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="56" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" s="13" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E3" s="14" t="n">
         <v>1</v>
@@ -2867,18 +2958,18 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>2</v>
@@ -2887,18 +2978,18 @@
         <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>3</v>
@@ -2907,15 +2998,15 @@
         <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>4</v>
@@ -2924,21 +3015,21 @@
         <v>1</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>5</v>
@@ -2947,21 +3038,21 @@
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>6</v>
@@ -2970,21 +3061,21 @@
         <v>1</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>7</v>
@@ -2993,18 +3084,18 @@
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>8</v>
@@ -3013,18 +3104,18 @@
         <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>9</v>
@@ -3035,13 +3126,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>10</v>
@@ -3050,15 +3141,15 @@
         <v>1</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>11</v>
@@ -3067,18 +3158,18 @@
         <v>1</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>12</v>
@@ -3087,12 +3178,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>